<commit_message>
Updated FIN model - 2025-08-28 17:12
</commit_message>
<xml_diff>
--- a/VerveStacks_FIN/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_FIN/ReportDefs_vervestacks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31B8C24-DE1E-41D4-9D22-F5A972B7FF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5A88F4-A9F3-4492-B398-74036C1411C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenMap" sheetId="56" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="265">
   <si>
     <t>Unit</t>
   </si>
@@ -458,9 +458,6 @@
     <t>old</t>
   </si>
   <si>
-    <t>ngfs</t>
-  </si>
-  <si>
     <t>timeslice</t>
   </si>
   <si>
@@ -566,9 +563,6 @@
     <t>-ElcAgg*,-*EV*,-g[_]*</t>
   </si>
   <si>
-    <t>ELC,ELC_???-???,e[_]*</t>
-  </si>
-  <si>
     <t>T_neg_andor</t>
   </si>
   <si>
@@ -788,21 +782,6 @@
     <t>Transformers Up</t>
   </si>
   <si>
-    <t>Declared NDCs</t>
-  </si>
-  <si>
-    <t>Limited to 2 deg</t>
-  </si>
-  <si>
-    <t>Postponed Transition</t>
-  </si>
-  <si>
-    <t>Target Net Zero 2050</t>
-  </si>
-  <si>
-    <t>Current Policies</t>
-  </si>
-  <si>
     <t>s1p1v1_d</t>
   </si>
   <si>
@@ -861,6 +840,42 @@
   </si>
   <si>
     <t>jAnn</t>
+  </si>
+  <si>
+    <t>Limit warming to 1.5°C (&gt;50%) with no or limited overshoot</t>
+  </si>
+  <si>
+    <t>Limit warming to 1.5°C (&gt;67%) with high overshoot</t>
+  </si>
+  <si>
+    <t>Limit warming to 2°C (&gt;67%) with higher action post-2030</t>
+  </si>
+  <si>
+    <t>Limit warming to 2°C (&gt;50%) with immediate action</t>
+  </si>
+  <si>
+    <t>Likely above 3°C warming with limited mitigation</t>
+  </si>
+  <si>
+    <t>b 2 deg (50%)</t>
+  </si>
+  <si>
+    <t>c 2 deg (67%)</t>
+  </si>
+  <si>
+    <t>d 1.5 deg OS</t>
+  </si>
+  <si>
+    <t>e 1.5 deg no OS</t>
+  </si>
+  <si>
+    <t>a 3 deg</t>
+  </si>
+  <si>
+    <t>ar6_r10</t>
+  </si>
+  <si>
+    <t>ELC,ELC_???-???*,e[_]*</t>
   </si>
 </sst>
 </file>
@@ -1407,8 +1422,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.73046875" defaultRowHeight="14.25"/>
@@ -1431,10 +1446,10 @@
     </row>
     <row r="2" spans="1:21">
       <c r="I2" t="s">
+        <v>263</v>
+      </c>
+      <c r="J2" t="s">
         <v>125</v>
-      </c>
-      <c r="J2" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -1466,7 +1481,7 @@
       </c>
       <c r="I5" t="str">
         <f>"sg_"&amp;I2</f>
-        <v>sg_ngfs</v>
+        <v>sg_ar6_r10</v>
       </c>
       <c r="J5" t="str">
         <f>"sg_"&amp;J2</f>
@@ -1483,19 +1498,22 @@
       </c>
       <c r="C6" t="str">
         <f>H6</f>
-        <v>Postponed Transition.e3d</v>
+        <v>e 1.5 deg no OS.e3d</v>
       </c>
       <c r="H6" t="str">
         <f>_xlfn.TEXTJOIN(".",TRUE,I6:J6)</f>
-        <v>Postponed Transition.e3d</v>
+        <v>e 1.5 deg no OS.e3d</v>
       </c>
       <c r="I6" t="s">
-        <v>237</v>
+        <v>261</v>
       </c>
       <c r="J6" t="str">
         <f>Q6</f>
         <v>e3d</v>
       </c>
+      <c r="L6" t="s">
+        <v>253</v>
+      </c>
       <c r="O6">
         <v>1</v>
       </c>
@@ -1507,10 +1525,10 @@
         <v>1</v>
       </c>
       <c r="T6" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="U6" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -1523,19 +1541,22 @@
       </c>
       <c r="C7" t="str">
         <f t="shared" ref="C7:C26" si="1">H7</f>
-        <v>Target Net Zero 2050.e3d</v>
+        <v>d 1.5 deg OS.e3d</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" ref="H7:H55" si="2">_xlfn.TEXTJOIN(".",TRUE,I7:J7)</f>
-        <v>Target Net Zero 2050.e3d</v>
+        <v>d 1.5 deg OS.e3d</v>
       </c>
       <c r="I7" t="s">
-        <v>238</v>
+        <v>260</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" ref="J7:J55" si="3">Q7</f>
         <v>e3d</v>
       </c>
+      <c r="L7" t="s">
+        <v>254</v>
+      </c>
       <c r="O7">
         <v>2</v>
       </c>
@@ -1547,10 +1568,10 @@
         <v>2</v>
       </c>
       <c r="T7" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="U7" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -1563,19 +1584,22 @@
       </c>
       <c r="C8" t="str">
         <f t="shared" si="1"/>
-        <v>Declared NDCs.e3d</v>
+        <v>c 2 deg (67%).e3d</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="2"/>
-        <v>Declared NDCs.e3d</v>
+        <v>c 2 deg (67%).e3d</v>
       </c>
       <c r="I8" t="s">
-        <v>235</v>
+        <v>259</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="3"/>
         <v>e3d</v>
       </c>
+      <c r="L8" t="s">
+        <v>255</v>
+      </c>
       <c r="O8">
         <v>3</v>
       </c>
@@ -1587,10 +1611,10 @@
         <v>3</v>
       </c>
       <c r="T8" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="U8" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -1603,19 +1627,22 @@
       </c>
       <c r="C9" t="str">
         <f t="shared" si="1"/>
-        <v>Limited to 2 deg.e3d</v>
+        <v>b 2 deg (50%).e3d</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="2"/>
-        <v>Limited to 2 deg.e3d</v>
+        <v>b 2 deg (50%).e3d</v>
       </c>
       <c r="I9" t="s">
-        <v>236</v>
+        <v>258</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="3"/>
         <v>e3d</v>
       </c>
+      <c r="L9" t="s">
+        <v>256</v>
+      </c>
       <c r="O9">
         <v>4</v>
       </c>
@@ -1627,10 +1654,10 @@
         <v>4</v>
       </c>
       <c r="T9" t="s">
+        <v>236</v>
+      </c>
+      <c r="U9" t="s">
         <v>243</v>
-      </c>
-      <c r="U9" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -1643,19 +1670,22 @@
       </c>
       <c r="C10" t="str">
         <f t="shared" si="1"/>
-        <v>Current Policies.e3d</v>
+        <v>a 3 deg.e3d</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="2"/>
-        <v>Current Policies.e3d</v>
+        <v>a 3 deg.e3d</v>
       </c>
       <c r="I10" t="s">
-        <v>239</v>
+        <v>262</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="3"/>
         <v>e3d</v>
       </c>
+      <c r="L10" t="s">
+        <v>257</v>
+      </c>
       <c r="O10">
         <v>5</v>
       </c>
@@ -1667,10 +1697,10 @@
         <v>5</v>
       </c>
       <c r="T10" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="U10" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1684,15 +1714,15 @@
       </c>
       <c r="C11" t="str">
         <f t="shared" si="1"/>
-        <v>Postponed Transition.d9d</v>
+        <v>e 1.5 deg no OS.d9d</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="2"/>
-        <v>Postponed Transition.d9d</v>
+        <v>e 1.5 deg no OS.d9d</v>
       </c>
       <c r="I11" t="str">
         <f>I6</f>
-        <v>Postponed Transition</v>
+        <v>e 1.5 deg no OS</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="3"/>
@@ -1710,10 +1740,10 @@
         <v>6</v>
       </c>
       <c r="T11" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="U11" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1727,15 +1757,15 @@
       </c>
       <c r="C12" t="str">
         <f t="shared" si="1"/>
-        <v>Target Net Zero 2050.d9d</v>
+        <v>d 1.5 deg OS.d9d</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="2"/>
-        <v>Target Net Zero 2050.d9d</v>
+        <v>d 1.5 deg OS.d9d</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" ref="I12:I55" si="6">I7</f>
-        <v>Target Net Zero 2050</v>
+        <v>d 1.5 deg OS</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="3"/>
@@ -1753,10 +1783,10 @@
         <v>7</v>
       </c>
       <c r="T12" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="U12" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1770,15 +1800,15 @@
       </c>
       <c r="C13" t="str">
         <f t="shared" si="1"/>
-        <v>Declared NDCs.d9d</v>
+        <v>c 2 deg (67%).d9d</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="2"/>
-        <v>Declared NDCs.d9d</v>
+        <v>c 2 deg (67%).d9d</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="6"/>
-        <v>Declared NDCs</v>
+        <v>c 2 deg (67%)</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="3"/>
@@ -1796,10 +1826,10 @@
         <v>8</v>
       </c>
       <c r="T13" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="U13" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1813,15 +1843,15 @@
       </c>
       <c r="C14" t="str">
         <f t="shared" si="1"/>
-        <v>Limited to 2 deg.d9d</v>
+        <v>b 2 deg (50%).d9d</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="2"/>
-        <v>Limited to 2 deg.d9d</v>
+        <v>b 2 deg (50%).d9d</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="6"/>
-        <v>Limited to 2 deg</v>
+        <v>b 2 deg (50%)</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="3"/>
@@ -1839,10 +1869,10 @@
         <v>9</v>
       </c>
       <c r="T14" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="U14" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1856,15 +1886,15 @@
       </c>
       <c r="C15" t="str">
         <f t="shared" si="1"/>
-        <v>Current Policies.d9d</v>
+        <v>a 3 deg.d9d</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="2"/>
-        <v>Current Policies.d9d</v>
+        <v>a 3 deg.d9d</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="6"/>
-        <v>Current Policies</v>
+        <v>a 3 deg</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="3"/>
@@ -1882,10 +1912,10 @@
         <v>10</v>
       </c>
       <c r="T15" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="U15" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -1899,15 +1929,15 @@
       </c>
       <c r="C16" t="str">
         <f t="shared" si="1"/>
-        <v>Postponed Transition.b2w</v>
+        <v>e 1.5 deg no OS.b2w</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="2"/>
-        <v>Postponed Transition.b2w</v>
+        <v>e 1.5 deg no OS.b2w</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="6"/>
-        <v>Postponed Transition</v>
+        <v>e 1.5 deg no OS</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="3"/>
@@ -1933,15 +1963,15 @@
       </c>
       <c r="C17" t="str">
         <f t="shared" si="1"/>
-        <v>Target Net Zero 2050.b2w</v>
+        <v>d 1.5 deg OS.b2w</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="2"/>
-        <v>Target Net Zero 2050.b2w</v>
+        <v>d 1.5 deg OS.b2w</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="6"/>
-        <v>Target Net Zero 2050</v>
+        <v>d 1.5 deg OS</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="3"/>
@@ -1967,15 +1997,15 @@
       </c>
       <c r="C18" t="str">
         <f t="shared" si="1"/>
-        <v>Declared NDCs.b2w</v>
+        <v>c 2 deg (67%).b2w</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="2"/>
-        <v>Declared NDCs.b2w</v>
+        <v>c 2 deg (67%).b2w</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" si="6"/>
-        <v>Declared NDCs</v>
+        <v>c 2 deg (67%)</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="3"/>
@@ -2001,15 +2031,15 @@
       </c>
       <c r="C19" t="str">
         <f t="shared" si="1"/>
-        <v>Limited to 2 deg.b2w</v>
+        <v>b 2 deg (50%).b2w</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="2"/>
-        <v>Limited to 2 deg.b2w</v>
+        <v>b 2 deg (50%).b2w</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="6"/>
-        <v>Limited to 2 deg</v>
+        <v>b 2 deg (50%)</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="3"/>
@@ -2035,15 +2065,15 @@
       </c>
       <c r="C20" t="str">
         <f t="shared" si="1"/>
-        <v>Current Policies.b2w</v>
+        <v>a 3 deg.b2w</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="2"/>
-        <v>Current Policies.b2w</v>
+        <v>a 3 deg.b2w</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="6"/>
-        <v>Current Policies</v>
+        <v>a 3 deg</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="3"/>
@@ -2069,15 +2099,15 @@
       </c>
       <c r="C21" t="str">
         <f t="shared" si="1"/>
-        <v>Postponed Transition.a2w2d</v>
+        <v>e 1.5 deg no OS.a2w2d</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="2"/>
-        <v>Postponed Transition.a2w2d</v>
+        <v>e 1.5 deg no OS.a2w2d</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="6"/>
-        <v>Postponed Transition</v>
+        <v>e 1.5 deg no OS</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="3"/>
@@ -2103,15 +2133,15 @@
       </c>
       <c r="C22" t="str">
         <f t="shared" si="1"/>
-        <v>Target Net Zero 2050.a2w2d</v>
+        <v>d 1.5 deg OS.a2w2d</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="2"/>
-        <v>Target Net Zero 2050.a2w2d</v>
+        <v>d 1.5 deg OS.a2w2d</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="6"/>
-        <v>Target Net Zero 2050</v>
+        <v>d 1.5 deg OS</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="3"/>
@@ -2137,15 +2167,15 @@
       </c>
       <c r="C23" t="str">
         <f t="shared" si="1"/>
-        <v>Declared NDCs.a2w2d</v>
+        <v>c 2 deg (67%).a2w2d</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="2"/>
-        <v>Declared NDCs.a2w2d</v>
+        <v>c 2 deg (67%).a2w2d</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="6"/>
-        <v>Declared NDCs</v>
+        <v>c 2 deg (67%)</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="3"/>
@@ -2171,15 +2201,15 @@
       </c>
       <c r="C24" t="str">
         <f t="shared" si="1"/>
-        <v>Limited to 2 deg.a2w2d</v>
+        <v>b 2 deg (50%).a2w2d</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="2"/>
-        <v>Limited to 2 deg.a2w2d</v>
+        <v>b 2 deg (50%).a2w2d</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="6"/>
-        <v>Limited to 2 deg</v>
+        <v>b 2 deg (50%)</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="3"/>
@@ -2205,15 +2235,15 @@
       </c>
       <c r="C25" t="str">
         <f t="shared" si="1"/>
-        <v>Current Policies.a2w2d</v>
+        <v>a 3 deg.a2w2d</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="2"/>
-        <v>Current Policies.a2w2d</v>
+        <v>a 3 deg.a2w2d</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="6"/>
-        <v>Current Policies</v>
+        <v>a 3 deg</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="3"/>
@@ -2239,15 +2269,15 @@
       </c>
       <c r="C26" t="str">
         <f t="shared" si="1"/>
-        <v>Postponed Transition.hTS12c</v>
+        <v>e 1.5 deg no OS.hTS12c</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="2"/>
-        <v>Postponed Transition.hTS12c</v>
+        <v>e 1.5 deg no OS.hTS12c</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="6"/>
-        <v>Postponed Transition</v>
+        <v>e 1.5 deg no OS</v>
       </c>
       <c r="J26" t="str">
         <f t="shared" si="3"/>
@@ -2273,15 +2303,15 @@
       </c>
       <c r="C27" t="str">
         <f t="shared" ref="C27:C40" si="8">H27</f>
-        <v>Target Net Zero 2050.hTS12c</v>
+        <v>d 1.5 deg OS.hTS12c</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="2"/>
-        <v>Target Net Zero 2050.hTS12c</v>
+        <v>d 1.5 deg OS.hTS12c</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="6"/>
-        <v>Target Net Zero 2050</v>
+        <v>d 1.5 deg OS</v>
       </c>
       <c r="J27" t="str">
         <f t="shared" si="3"/>
@@ -2307,15 +2337,15 @@
       </c>
       <c r="C28" t="str">
         <f t="shared" si="8"/>
-        <v>Declared NDCs.hTS12c</v>
+        <v>c 2 deg (67%).hTS12c</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="2"/>
-        <v>Declared NDCs.hTS12c</v>
+        <v>c 2 deg (67%).hTS12c</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="6"/>
-        <v>Declared NDCs</v>
+        <v>c 2 deg (67%)</v>
       </c>
       <c r="J28" t="str">
         <f t="shared" si="3"/>
@@ -2341,15 +2371,15 @@
       </c>
       <c r="C29" t="str">
         <f t="shared" si="8"/>
-        <v>Limited to 2 deg.hTS12c</v>
+        <v>b 2 deg (50%).hTS12c</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="2"/>
-        <v>Limited to 2 deg.hTS12c</v>
+        <v>b 2 deg (50%).hTS12c</v>
       </c>
       <c r="I29" t="str">
         <f t="shared" si="6"/>
-        <v>Limited to 2 deg</v>
+        <v>b 2 deg (50%)</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="3"/>
@@ -2375,15 +2405,15 @@
       </c>
       <c r="C30" t="str">
         <f t="shared" si="8"/>
-        <v>Current Policies.hTS12c</v>
+        <v>a 3 deg.hTS12c</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="2"/>
-        <v>Current Policies.hTS12c</v>
+        <v>a 3 deg.hTS12c</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" si="6"/>
-        <v>Current Policies</v>
+        <v>a 3 deg</v>
       </c>
       <c r="J30" t="str">
         <f t="shared" si="3"/>
@@ -2409,15 +2439,15 @@
       </c>
       <c r="C31" t="str">
         <f t="shared" si="8"/>
-        <v>Postponed Transition.gTS24c</v>
+        <v>e 1.5 deg no OS.gTS24c</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="2"/>
-        <v>Postponed Transition.gTS24c</v>
+        <v>e 1.5 deg no OS.gTS24c</v>
       </c>
       <c r="I31" t="str">
         <f t="shared" si="6"/>
-        <v>Postponed Transition</v>
+        <v>e 1.5 deg no OS</v>
       </c>
       <c r="J31" t="str">
         <f t="shared" si="3"/>
@@ -2443,15 +2473,15 @@
       </c>
       <c r="C32" t="str">
         <f t="shared" si="8"/>
-        <v>Target Net Zero 2050.gTS24c</v>
+        <v>d 1.5 deg OS.gTS24c</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="2"/>
-        <v>Target Net Zero 2050.gTS24c</v>
+        <v>d 1.5 deg OS.gTS24c</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" si="6"/>
-        <v>Target Net Zero 2050</v>
+        <v>d 1.5 deg OS</v>
       </c>
       <c r="J32" t="str">
         <f t="shared" si="3"/>
@@ -2477,15 +2507,15 @@
       </c>
       <c r="C33" t="str">
         <f t="shared" si="8"/>
-        <v>Declared NDCs.gTS24c</v>
+        <v>c 2 deg (67%).gTS24c</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="2"/>
-        <v>Declared NDCs.gTS24c</v>
+        <v>c 2 deg (67%).gTS24c</v>
       </c>
       <c r="I33" t="str">
         <f t="shared" si="6"/>
-        <v>Declared NDCs</v>
+        <v>c 2 deg (67%)</v>
       </c>
       <c r="J33" t="str">
         <f t="shared" si="3"/>
@@ -2511,15 +2541,15 @@
       </c>
       <c r="C34" t="str">
         <f t="shared" si="8"/>
-        <v>Limited to 2 deg.gTS24c</v>
+        <v>b 2 deg (50%).gTS24c</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="2"/>
-        <v>Limited to 2 deg.gTS24c</v>
+        <v>b 2 deg (50%).gTS24c</v>
       </c>
       <c r="I34" t="str">
         <f t="shared" si="6"/>
-        <v>Limited to 2 deg</v>
+        <v>b 2 deg (50%)</v>
       </c>
       <c r="J34" t="str">
         <f t="shared" si="3"/>
@@ -2545,15 +2575,15 @@
       </c>
       <c r="C35" t="str">
         <f t="shared" si="8"/>
-        <v>Current Policies.gTS24c</v>
+        <v>a 3 deg.gTS24c</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="2"/>
-        <v>Current Policies.gTS24c</v>
+        <v>a 3 deg.gTS24c</v>
       </c>
       <c r="I35" t="str">
         <f t="shared" si="6"/>
-        <v>Current Policies</v>
+        <v>a 3 deg</v>
       </c>
       <c r="J35" t="str">
         <f t="shared" si="3"/>
@@ -2579,15 +2609,15 @@
       </c>
       <c r="C36" t="str">
         <f t="shared" si="8"/>
-        <v>Postponed Transition.fTS48c</v>
+        <v>e 1.5 deg no OS.fTS48c</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="2"/>
-        <v>Postponed Transition.fTS48c</v>
+        <v>e 1.5 deg no OS.fTS48c</v>
       </c>
       <c r="I36" t="str">
         <f t="shared" si="6"/>
-        <v>Postponed Transition</v>
+        <v>e 1.5 deg no OS</v>
       </c>
       <c r="J36" t="str">
         <f t="shared" si="3"/>
@@ -2613,15 +2643,15 @@
       </c>
       <c r="C37" t="str">
         <f t="shared" si="8"/>
-        <v>Target Net Zero 2050.fTS48c</v>
+        <v>d 1.5 deg OS.fTS48c</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="2"/>
-        <v>Target Net Zero 2050.fTS48c</v>
+        <v>d 1.5 deg OS.fTS48c</v>
       </c>
       <c r="I37" t="str">
         <f t="shared" si="6"/>
-        <v>Target Net Zero 2050</v>
+        <v>d 1.5 deg OS</v>
       </c>
       <c r="J37" t="str">
         <f t="shared" si="3"/>
@@ -2642,20 +2672,20 @@
         <v>7</v>
       </c>
       <c r="B38" t="str">
-        <f t="shared" ref="B38:B69" si="9">"vstacks_"&amp;VLOOKUP(A38,$S$6:$T$18,2,FALSE)&amp;"~"&amp;TEXT(O38,"0000")</f>
+        <f t="shared" ref="B38:B55" si="9">"vstacks_"&amp;VLOOKUP(A38,$S$6:$T$18,2,FALSE)&amp;"~"&amp;TEXT(O38,"0000")</f>
         <v>vstacks_ts48_clu~0003</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="8"/>
-        <v>Declared NDCs.fTS48c</v>
+        <v>c 2 deg (67%).fTS48c</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="2"/>
-        <v>Declared NDCs.fTS48c</v>
+        <v>c 2 deg (67%).fTS48c</v>
       </c>
       <c r="I38" t="str">
         <f t="shared" si="6"/>
-        <v>Declared NDCs</v>
+        <v>c 2 deg (67%)</v>
       </c>
       <c r="J38" t="str">
         <f t="shared" si="3"/>
@@ -2681,15 +2711,15 @@
       </c>
       <c r="C39" t="str">
         <f t="shared" si="8"/>
-        <v>Limited to 2 deg.fTS48c</v>
+        <v>b 2 deg (50%).fTS48c</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="2"/>
-        <v>Limited to 2 deg.fTS48c</v>
+        <v>b 2 deg (50%).fTS48c</v>
       </c>
       <c r="I39" t="str">
         <f t="shared" si="6"/>
-        <v>Limited to 2 deg</v>
+        <v>b 2 deg (50%)</v>
       </c>
       <c r="J39" t="str">
         <f t="shared" si="3"/>
@@ -2715,15 +2745,15 @@
       </c>
       <c r="C40" t="str">
         <f t="shared" si="8"/>
-        <v>Current Policies.fTS48c</v>
+        <v>a 3 deg.fTS48c</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="2"/>
-        <v>Current Policies.fTS48c</v>
+        <v>a 3 deg.fTS48c</v>
       </c>
       <c r="I40" t="str">
         <f t="shared" si="6"/>
-        <v>Current Policies</v>
+        <v>a 3 deg</v>
       </c>
       <c r="J40" t="str">
         <f t="shared" si="3"/>
@@ -2749,15 +2779,15 @@
       </c>
       <c r="C41" t="str">
         <f t="shared" ref="C41:C55" si="10">H41</f>
-        <v>Postponed Transition.c15d</v>
+        <v>e 1.5 deg no OS.c15d</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="2"/>
-        <v>Postponed Transition.c15d</v>
+        <v>e 1.5 deg no OS.c15d</v>
       </c>
       <c r="I41" t="str">
         <f t="shared" si="6"/>
-        <v>Postponed Transition</v>
+        <v>e 1.5 deg no OS</v>
       </c>
       <c r="J41" t="str">
         <f t="shared" si="3"/>
@@ -2783,15 +2813,15 @@
       </c>
       <c r="C42" t="str">
         <f t="shared" si="10"/>
-        <v>Target Net Zero 2050.c15d</v>
+        <v>d 1.5 deg OS.c15d</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="2"/>
-        <v>Target Net Zero 2050.c15d</v>
+        <v>d 1.5 deg OS.c15d</v>
       </c>
       <c r="I42" t="str">
         <f t="shared" si="6"/>
-        <v>Target Net Zero 2050</v>
+        <v>d 1.5 deg OS</v>
       </c>
       <c r="J42" t="str">
         <f t="shared" si="3"/>
@@ -2817,15 +2847,15 @@
       </c>
       <c r="C43" t="str">
         <f t="shared" si="10"/>
-        <v>Declared NDCs.c15d</v>
+        <v>c 2 deg (67%).c15d</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="2"/>
-        <v>Declared NDCs.c15d</v>
+        <v>c 2 deg (67%).c15d</v>
       </c>
       <c r="I43" t="str">
         <f t="shared" si="6"/>
-        <v>Declared NDCs</v>
+        <v>c 2 deg (67%)</v>
       </c>
       <c r="J43" t="str">
         <f t="shared" si="3"/>
@@ -2851,15 +2881,15 @@
       </c>
       <c r="C44" t="str">
         <f t="shared" si="10"/>
-        <v>Limited to 2 deg.c15d</v>
+        <v>b 2 deg (50%).c15d</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="2"/>
-        <v>Limited to 2 deg.c15d</v>
+        <v>b 2 deg (50%).c15d</v>
       </c>
       <c r="I44" t="str">
         <f t="shared" si="6"/>
-        <v>Limited to 2 deg</v>
+        <v>b 2 deg (50%)</v>
       </c>
       <c r="J44" t="str">
         <f t="shared" si="3"/>
@@ -2885,15 +2915,15 @@
       </c>
       <c r="C45" t="str">
         <f t="shared" si="10"/>
-        <v>Current Policies.c15d</v>
+        <v>a 3 deg.c15d</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="2"/>
-        <v>Current Policies.c15d</v>
+        <v>a 3 deg.c15d</v>
       </c>
       <c r="I45" t="str">
         <f t="shared" si="6"/>
-        <v>Current Policies</v>
+        <v>a 3 deg</v>
       </c>
       <c r="J45" t="str">
         <f t="shared" si="3"/>
@@ -2919,15 +2949,15 @@
       </c>
       <c r="C46" t="str">
         <f t="shared" si="10"/>
-        <v>Postponed Transition.iTS12</v>
+        <v>e 1.5 deg no OS.iTS12</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="2"/>
-        <v>Postponed Transition.iTS12</v>
+        <v>e 1.5 deg no OS.iTS12</v>
       </c>
       <c r="I46" t="str">
         <f t="shared" si="6"/>
-        <v>Postponed Transition</v>
+        <v>e 1.5 deg no OS</v>
       </c>
       <c r="J46" t="str">
         <f t="shared" si="3"/>
@@ -2953,15 +2983,15 @@
       </c>
       <c r="C47" t="str">
         <f t="shared" si="10"/>
-        <v>Target Net Zero 2050.iTS12</v>
+        <v>d 1.5 deg OS.iTS12</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="2"/>
-        <v>Target Net Zero 2050.iTS12</v>
+        <v>d 1.5 deg OS.iTS12</v>
       </c>
       <c r="I47" t="str">
         <f t="shared" si="6"/>
-        <v>Target Net Zero 2050</v>
+        <v>d 1.5 deg OS</v>
       </c>
       <c r="J47" t="str">
         <f t="shared" si="3"/>
@@ -2987,15 +3017,15 @@
       </c>
       <c r="C48" t="str">
         <f t="shared" si="10"/>
-        <v>Declared NDCs.iTS12</v>
+        <v>c 2 deg (67%).iTS12</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="2"/>
-        <v>Declared NDCs.iTS12</v>
+        <v>c 2 deg (67%).iTS12</v>
       </c>
       <c r="I48" t="str">
         <f t="shared" si="6"/>
-        <v>Declared NDCs</v>
+        <v>c 2 deg (67%)</v>
       </c>
       <c r="J48" t="str">
         <f t="shared" si="3"/>
@@ -3021,15 +3051,15 @@
       </c>
       <c r="C49" t="str">
         <f t="shared" si="10"/>
-        <v>Limited to 2 deg.iTS12</v>
+        <v>b 2 deg (50%).iTS12</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="2"/>
-        <v>Limited to 2 deg.iTS12</v>
+        <v>b 2 deg (50%).iTS12</v>
       </c>
       <c r="I49" t="str">
         <f t="shared" si="6"/>
-        <v>Limited to 2 deg</v>
+        <v>b 2 deg (50%)</v>
       </c>
       <c r="J49" t="str">
         <f t="shared" si="3"/>
@@ -3055,15 +3085,15 @@
       </c>
       <c r="C50" t="str">
         <f t="shared" si="10"/>
-        <v>Current Policies.iTS12</v>
+        <v>a 3 deg.iTS12</v>
       </c>
       <c r="H50" t="str">
         <f t="shared" si="2"/>
-        <v>Current Policies.iTS12</v>
+        <v>a 3 deg.iTS12</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" si="6"/>
-        <v>Current Policies</v>
+        <v>a 3 deg</v>
       </c>
       <c r="J50" t="str">
         <f t="shared" si="3"/>
@@ -3089,15 +3119,15 @@
       </c>
       <c r="C51" t="str">
         <f t="shared" si="10"/>
-        <v>Postponed Transition.jAnn</v>
+        <v>e 1.5 deg no OS.jAnn</v>
       </c>
       <c r="H51" t="str">
         <f t="shared" si="2"/>
-        <v>Postponed Transition.jAnn</v>
+        <v>e 1.5 deg no OS.jAnn</v>
       </c>
       <c r="I51" t="str">
         <f t="shared" si="6"/>
-        <v>Postponed Transition</v>
+        <v>e 1.5 deg no OS</v>
       </c>
       <c r="J51" t="str">
         <f t="shared" si="3"/>
@@ -3123,15 +3153,15 @@
       </c>
       <c r="C52" t="str">
         <f t="shared" si="10"/>
-        <v>Target Net Zero 2050.jAnn</v>
+        <v>d 1.5 deg OS.jAnn</v>
       </c>
       <c r="H52" t="str">
         <f t="shared" si="2"/>
-        <v>Target Net Zero 2050.jAnn</v>
+        <v>d 1.5 deg OS.jAnn</v>
       </c>
       <c r="I52" t="str">
         <f t="shared" si="6"/>
-        <v>Target Net Zero 2050</v>
+        <v>d 1.5 deg OS</v>
       </c>
       <c r="J52" t="str">
         <f t="shared" si="3"/>
@@ -3157,15 +3187,15 @@
       </c>
       <c r="C53" t="str">
         <f t="shared" si="10"/>
-        <v>Declared NDCs.jAnn</v>
+        <v>c 2 deg (67%).jAnn</v>
       </c>
       <c r="H53" t="str">
         <f t="shared" si="2"/>
-        <v>Declared NDCs.jAnn</v>
+        <v>c 2 deg (67%).jAnn</v>
       </c>
       <c r="I53" t="str">
         <f t="shared" si="6"/>
-        <v>Declared NDCs</v>
+        <v>c 2 deg (67%)</v>
       </c>
       <c r="J53" t="str">
         <f t="shared" si="3"/>
@@ -3191,15 +3221,15 @@
       </c>
       <c r="C54" t="str">
         <f t="shared" si="10"/>
-        <v>Limited to 2 deg.jAnn</v>
+        <v>b 2 deg (50%).jAnn</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="2"/>
-        <v>Limited to 2 deg.jAnn</v>
+        <v>b 2 deg (50%).jAnn</v>
       </c>
       <c r="I54" t="str">
         <f t="shared" si="6"/>
-        <v>Limited to 2 deg</v>
+        <v>b 2 deg (50%)</v>
       </c>
       <c r="J54" t="str">
         <f t="shared" si="3"/>
@@ -3225,15 +3255,15 @@
       </c>
       <c r="C55" t="str">
         <f t="shared" si="10"/>
-        <v>Current Policies.jAnn</v>
+        <v>a 3 deg.jAnn</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="2"/>
-        <v>Current Policies.jAnn</v>
+        <v>a 3 deg.jAnn</v>
       </c>
       <c r="I55" t="str">
         <f t="shared" si="6"/>
-        <v>Current Policies</v>
+        <v>a 3 deg</v>
       </c>
       <c r="J55" t="str">
         <f t="shared" si="3"/>
@@ -3436,10 +3466,10 @@
         <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D5">
         <v>1E-3</v>
@@ -3450,10 +3480,10 @@
         <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D6">
         <v>-1E-3</v>
@@ -3464,10 +3494,10 @@
         <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D7">
         <v>-1000</v>
@@ -3483,9 +3513,9 @@
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -3583,7 +3613,7 @@
         <v>116</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K3" t="s">
         <v>8</v>
@@ -3600,7 +3630,7 @@
         <v>116</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K4" t="s">
         <v>8</v>
@@ -3621,10 +3651,10 @@
         <v>117</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I5" t="s">
-        <v>161</v>
+        <v>264</v>
       </c>
       <c r="K5" t="s">
         <v>81</v>
@@ -3644,7 +3674,7 @@
         <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D6" s="2"/>
       <c r="H6" t="s">
@@ -3670,13 +3700,13 @@
         <v>5</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
@@ -3686,13 +3716,13 @@
         <v>5</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
@@ -3745,13 +3775,13 @@
         <v>57</v>
       </c>
       <c r="I11" t="s">
+        <v>141</v>
+      </c>
+      <c r="K11" t="s">
         <v>142</v>
       </c>
-      <c r="K11" t="s">
+      <c r="N11" t="s">
         <v>143</v>
-      </c>
-      <c r="N11" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -3915,7 +3945,7 @@
   <sheetData>
     <row r="3" spans="1:19" ht="17.25" thickBot="1">
       <c r="A3" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15" thickTop="1" thickBot="1">
@@ -3971,10 +4001,10 @@
         <v>107</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -3990,10 +4020,10 @@
         <v>Elec-220V,Elec-400V,Elec-380V,Elec-225V,Elec-330V,Elec-275V,Elec-420V,Elec-300V,Elec-500V,Elec-750V,Elec-450V,Elec-515V,Elec-525V,Elec-320V,Elec-150V,Elec-270V,Elec-350V,Elec-250V,Elec-200V,Elec-236V,Elec-600V,Solar elec,Wind elec,fossil,renewable,bioenergy,hydrogen,nuclear,ELC,buildings,industry,transport,EVs</v>
       </c>
       <c r="J5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="M5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="S5">
         <v>-1</v>
@@ -4001,7 +4031,7 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B6" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,PSet_MAP!$A$3:$A$49)</f>
@@ -4012,10 +4042,10 @@
         <v>Elec-220V,Elec-400V,Elec-380V,Elec-225V,Elec-330V,Elec-275V,Elec-420V,Elec-300V,Elec-500V,Elec-750V,Elec-450V,Elec-515V,Elec-525V,Elec-320V,Elec-150V,Elec-270V,Elec-350V,Elec-250V,Elec-200V,Elec-236V,Elec-600V,Solar elec,Wind elec,fossil,renewable,bioenergy,hydrogen,nuclear,ELC,buildings,industry,transport,EVs</v>
       </c>
       <c r="J6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="M6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="S6">
         <v>-1</v>
@@ -4123,7 +4153,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
@@ -4132,7 +4162,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
@@ -4159,7 +4189,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
@@ -4168,7 +4198,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
@@ -4177,7 +4207,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
@@ -4186,7 +4216,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
@@ -4195,7 +4225,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
@@ -4231,7 +4261,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
@@ -4240,7 +4270,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
@@ -4249,7 +4279,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
@@ -4258,7 +4288,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
@@ -4267,7 +4297,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
@@ -4276,7 +4306,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
@@ -4285,7 +4315,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
@@ -4294,7 +4324,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
@@ -4303,7 +4333,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
@@ -4312,7 +4342,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
@@ -4321,7 +4351,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
@@ -4330,7 +4360,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
@@ -4339,7 +4369,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="0"/>
@@ -4348,7 +4378,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
@@ -4357,7 +4387,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
@@ -4366,7 +4396,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
@@ -4375,7 +4405,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
@@ -4384,7 +4414,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
@@ -4393,7 +4423,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
@@ -4402,7 +4432,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
@@ -4411,7 +4441,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
@@ -4420,7 +4450,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
@@ -4429,7 +4459,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="0"/>
@@ -4438,7 +4468,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
@@ -4447,7 +4477,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
@@ -4456,7 +4486,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="0"/>
@@ -4500,7 +4530,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B3" t="str">
         <f>A3</f>
@@ -4509,7 +4539,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" ref="B4:B35" si="0">A4</f>
@@ -4518,7 +4548,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
@@ -4527,7 +4557,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
@@ -4536,7 +4566,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
@@ -4545,7 +4575,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
@@ -4554,7 +4584,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
@@ -4563,7 +4593,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
@@ -4572,7 +4602,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
@@ -4581,7 +4611,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
@@ -4590,7 +4620,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
@@ -4599,7 +4629,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
@@ -4608,7 +4638,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
@@ -4617,7 +4647,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
@@ -4626,7 +4656,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
@@ -4635,7 +4665,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
@@ -4644,7 +4674,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
@@ -4653,7 +4683,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
@@ -4662,7 +4692,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
@@ -4671,7 +4701,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
@@ -4680,7 +4710,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
@@ -4689,7 +4719,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
@@ -4698,7 +4728,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
@@ -4707,7 +4737,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
@@ -4716,7 +4746,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
@@ -4725,7 +4755,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
@@ -4734,7 +4764,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
@@ -4743,7 +4773,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
@@ -4752,7 +4782,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
@@ -4761,7 +4791,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
@@ -4770,7 +4800,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
@@ -4779,7 +4809,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="0"/>
@@ -4788,7 +4818,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
@@ -4858,7 +4888,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4874,32 +4904,32 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" t="s">
         <v>148</v>
-      </c>
-      <c r="C3" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" t="s">
         <v>152</v>
-      </c>
-      <c r="B5" t="s">
-        <v>153</v>
       </c>
       <c r="C5" t="str">
         <f>LEFT(B5,2)</f>
@@ -4908,10 +4938,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ref="C6:C10" si="0">LEFT(B6,2)</f>
@@ -4920,10 +4950,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -4932,10 +4962,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -4944,10 +4974,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -4956,10 +4986,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -5132,7 +5162,7 @@
         <v>Bio Power</v>
       </c>
       <c r="D12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -5144,7 +5174,7 @@
         <v>Solar Util</v>
       </c>
       <c r="D13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -5180,7 +5210,7 @@
         <v>Geothermal P</v>
       </c>
       <c r="D16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -5192,7 +5222,7 @@
         <v>Hydro Dam</v>
       </c>
       <c r="D17" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -5204,7 +5234,7 @@
         <v>Hydro RoR</v>
       </c>
       <c r="D18" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -5216,7 +5246,7 @@
         <v>Nuclear P</v>
       </c>
       <c r="D19" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -5228,7 +5258,7 @@
         <v>Nuclear SMR</v>
       </c>
       <c r="D20" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -5276,7 +5306,7 @@
         <v>Demand</v>
       </c>
       <c r="D24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5288,7 +5318,7 @@
         <v>Transformers Dn</v>
       </c>
       <c r="D25" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -5300,7 +5330,7 @@
         <v>Transformers Up</v>
       </c>
       <c r="D26" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -5312,7 +5342,7 @@
         <v>Grid-220V</v>
       </c>
       <c r="D27" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -5324,7 +5354,7 @@
         <v>Grid-400V</v>
       </c>
       <c r="D28" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5336,7 +5366,7 @@
         <v>Grid-380V</v>
       </c>
       <c r="D29" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -5348,7 +5378,7 @@
         <v>Grid-225V</v>
       </c>
       <c r="D30" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -5360,7 +5390,7 @@
         <v>Grid-330V</v>
       </c>
       <c r="D31" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -5372,7 +5402,7 @@
         <v>Grid-275V</v>
       </c>
       <c r="D32" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -5384,7 +5414,7 @@
         <v>Grid-420V</v>
       </c>
       <c r="D33" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -5396,7 +5426,7 @@
         <v>Grid-300V</v>
       </c>
       <c r="D34" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -5408,7 +5438,7 @@
         <v>Grid-500V</v>
       </c>
       <c r="D35" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -5420,7 +5450,7 @@
         <v>Grid-750V</v>
       </c>
       <c r="D36" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -5432,7 +5462,7 @@
         <v>Grid-450V</v>
       </c>
       <c r="D37" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -5444,7 +5474,7 @@
         <v>Grid-515V</v>
       </c>
       <c r="D38" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -5456,7 +5486,7 @@
         <v>Grid-525V</v>
       </c>
       <c r="D39" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -5468,7 +5498,7 @@
         <v>Grid-320V</v>
       </c>
       <c r="D40" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -5480,7 +5510,7 @@
         <v>Grid-150V</v>
       </c>
       <c r="D41" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -5492,7 +5522,7 @@
         <v>Grid-270V</v>
       </c>
       <c r="D42" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -5504,7 +5534,7 @@
         <v>Grid-350V</v>
       </c>
       <c r="D43" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -5516,7 +5546,7 @@
         <v>Grid-250V</v>
       </c>
       <c r="D44" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -5528,7 +5558,7 @@
         <v>Grid-200V</v>
       </c>
       <c r="D45" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -5540,7 +5570,7 @@
         <v>Grid-236V</v>
       </c>
       <c r="D46" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -5552,7 +5582,7 @@
         <v>Grid-600V</v>
       </c>
       <c r="D47" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -5564,7 +5594,7 @@
         <v>Aggregators</v>
       </c>
       <c r="D48" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -5576,7 +5606,7 @@
         <v>DUMMY_IMP</v>
       </c>
       <c r="D49" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -5584,13 +5614,13 @@
         <v>70</v>
       </c>
       <c r="C50" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E50" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F50" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -5598,13 +5628,13 @@
         <v>70</v>
       </c>
       <c r="C51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E51" t="s">
+        <v>138</v>
+      </c>
+      <c r="F51" t="s">
         <v>139</v>
-      </c>
-      <c r="F51" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -5612,13 +5642,13 @@
         <v>70</v>
       </c>
       <c r="B52" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C52" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E52" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -5626,13 +5656,13 @@
         <v>70</v>
       </c>
       <c r="B53" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C53" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E53" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:6">

</xml_diff>